<commit_message>
Descarga en excel solo backend
</commit_message>
<xml_diff>
--- a/movimientos.xlsx
+++ b/movimientos.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1,725,882.00</t>
+          <t>.00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>383,493.00</t>
+          <t>545,474,228.14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,200,000.00</t>
+          <t>1,570.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>909,375.00</t>
+          <t>545,472,658.14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>383,493.00</t>
+          <t>22,416.14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Version que produce excel
Falta mandarlo al front y boton de descarga
</commit_message>
<xml_diff>
--- a/movimientos.xlsx
+++ b/movimientos.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1,725,882.00</t>
+          <t>.00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>383,493.00</t>
+          <t>545,474,228.14</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,200,000.00</t>
+          <t>1,570.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>909,375.00</t>
+          <t>545,472,658.14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>383,493.00</t>
+          <t>22,416.14</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega endopint para descargar excel y lógica en el front, más estilos
</commit_message>
<xml_diff>
--- a/movimientos.xlsx
+++ b/movimientos.xlsx
@@ -463,27 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>.00</t>
+          <t>1,725,882.00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>545,474,228.14</t>
+          <t>383,493.00</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1,570.00</t>
+          <t>1,200,000.00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>545,472,658.14</t>
+          <t>909,375.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>22,416.14</t>
+          <t>383,493.00</t>
         </is>
       </c>
     </row>

</xml_diff>